<commit_message>
Add T1 bis to foyer convention
</commit_message>
<xml_diff>
--- a/static/files/foyer_residence_logements.xlsx
+++ b/static/files/foyer_residence_logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1179FB7C-3976-4A79-9DEB-6879445BA729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0F1DF-17BE-4A40-8C8D-D1106EC1C459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1400" yWindow="500" windowWidth="27400" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>T1</t>
+  </si>
+  <si>
+    <t>T1 bis</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A9" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A9" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A10" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A10" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de logement" dataDxfId="0"/>
   </tableColumns>
@@ -472,7 +475,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -771,16 +774,16 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.625" customWidth="1"/>
-    <col min="2" max="4" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="4" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -794,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>17</v>
       </c>
@@ -802,7 +805,7 @@
       <c r="C2" s="25"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="12"/>
@@ -811,7 +814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="11"/>
@@ -820,19 +823,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="12"/>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="11"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="12"/>
@@ -846,7 +849,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="11"/>
@@ -860,265 +863,265 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="12"/>
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="11"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="12"/>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="11"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="12"/>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="11"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="12"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="11"/>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="12"/>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="11"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="12"/>
       <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="11"/>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="12"/>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="11"/>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="12"/>
       <c r="D23" s="16"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="11"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="12"/>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="11"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="12"/>
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="11"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="12"/>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="11"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="12"/>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="11"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="12"/>
       <c r="D33" s="16"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="11"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="12"/>
       <c r="D35" s="16"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
       <c r="C36" s="11"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="12"/>
       <c r="D37" s="16"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="11"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="12"/>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="11"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="12"/>
       <c r="D41" s="16"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="11"/>
       <c r="D42" s="15"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="12"/>
       <c r="D43" s="16"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="11"/>
       <c r="D44" s="15"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="12"/>
       <c r="D45" s="16"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="11"/>
       <c r="D46" s="15"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="12"/>
       <c r="D47" s="16"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
       <c r="C48" s="11"/>
       <c r="D48" s="15"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="12"/>
       <c r="D49" s="16"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
       <c r="C50" s="11"/>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="12"/>
       <c r="D51" s="16"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="9"/>
       <c r="C52" s="13"/>
@@ -1138,7 +1141,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92FF0F08-53C6-4886-A5AA-66266516A04A}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$9</xm:f>
+            <xm:f>Data!$A$2:$A$10</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B52</xm:sqref>
         </x14:dataValidation>
@@ -1154,43 +1157,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1203,18 +1206,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1222,55 +1223,61 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E4" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pVHGyaqjpluKkGlcdUCwYGM0hS2GZZMKRlgRWh/5Pr1d9nT5aPo2/XkcvL3Hyr7ILNREV5Tvbh3REC+ZgmbKDw==" saltValue="feoIZrIll29OnV/4xJ8T4Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TyYFcPJH22iylfRKqcF4MUGl0BH/NQFdTkMG2R4weJjPZYlwxS9M0MULSbE0ioE+p9H7HcoHbSiVUzdOjorq4g==" saltValue="AfIcMrTXLf7yhfeYrWaK4g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add T1 bis to foyer convention (#492)
</commit_message>
<xml_diff>
--- a/static/files/foyer_residence_logements.xlsx
+++ b/static/files/foyer_residence_logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1179FB7C-3976-4A79-9DEB-6879445BA729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0F1DF-17BE-4A40-8C8D-D1106EC1C459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1400" yWindow="500" windowWidth="27400" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>T1</t>
+  </si>
+  <si>
+    <t>T1 bis</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A9" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A9" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A10" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A10" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de logement" dataDxfId="0"/>
   </tableColumns>
@@ -472,7 +475,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -771,16 +774,16 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.625" customWidth="1"/>
-    <col min="2" max="4" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="4" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -794,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>17</v>
       </c>
@@ -802,7 +805,7 @@
       <c r="C2" s="25"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="12"/>
@@ -811,7 +814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="11"/>
@@ -820,19 +823,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="12"/>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="11"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="12"/>
@@ -846,7 +849,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="11"/>
@@ -860,265 +863,265 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="12"/>
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="11"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="12"/>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="11"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="12"/>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="11"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="12"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="11"/>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="12"/>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="11"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="12"/>
       <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="11"/>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="12"/>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="11"/>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="12"/>
       <c r="D23" s="16"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="11"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="12"/>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="11"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="12"/>
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="11"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="12"/>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="11"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="12"/>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="11"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="12"/>
       <c r="D33" s="16"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="11"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="12"/>
       <c r="D35" s="16"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
       <c r="C36" s="11"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="12"/>
       <c r="D37" s="16"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="11"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="12"/>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="11"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="12"/>
       <c r="D41" s="16"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="11"/>
       <c r="D42" s="15"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="12"/>
       <c r="D43" s="16"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="11"/>
       <c r="D44" s="15"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="12"/>
       <c r="D45" s="16"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="11"/>
       <c r="D46" s="15"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="12"/>
       <c r="D47" s="16"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
       <c r="C48" s="11"/>
       <c r="D48" s="15"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="12"/>
       <c r="D49" s="16"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
       <c r="C50" s="11"/>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="12"/>
       <c r="D51" s="16"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="9"/>
       <c r="C52" s="13"/>
@@ -1138,7 +1141,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92FF0F08-53C6-4886-A5AA-66266516A04A}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$9</xm:f>
+            <xm:f>Data!$A$2:$A$10</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B52</xm:sqref>
         </x14:dataValidation>
@@ -1154,43 +1157,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1203,18 +1206,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1222,55 +1223,61 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E4" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pVHGyaqjpluKkGlcdUCwYGM0hS2GZZMKRlgRWh/5Pr1d9nT5aPo2/XkcvL3Hyr7ILNREV5Tvbh3REC+ZgmbKDw==" saltValue="feoIZrIll29OnV/4xJ8T4Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TyYFcPJH22iylfRKqcF4MUGl0BH/NQFdTkMG2R4weJjPZYlwxS9M0MULSbE0ioE+p9H7HcoHbSiVUzdOjorq4g==" saltValue="AfIcMrTXLf7yhfeYrWaK4g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>